<commit_message>
dmmd examen - 4 de 10
</commit_message>
<xml_diff>
--- a/Datos_Masivos/Verano_2023/ENGIN61901-2023A.xlsx
+++ b/Datos_Masivos/Verano_2023/ENGIN61901-2023A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andriu\Main\DOCUMENTOS\1. LABORALES\2. AYUDANTIAS\AyudantiasFEN\Datos_Masivos\Verano_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E29CF19-7E07-4A7B-A379-5764DC27EF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB34F48E-4059-4042-BE56-BBB47B57DEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{8460F878-2C6C-4FF6-8E48-E70BC54E4E5E}"/>
   </bookViews>
@@ -577,17 +577,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1181,11 +1181,11 @@
       </c>
       <c r="G9">
         <f>+VLOOKUP(A9,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
+        <v>6.25</v>
       </c>
       <c r="H9" s="9">
         <f t="shared" si="0"/>
-        <v>3.7</v>
+        <v>6.3250000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1214,11 +1214,11 @@
       </c>
       <c r="G10">
         <f>+VLOOKUP(A10,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
+        <v>6.625</v>
       </c>
       <c r="H10" s="9">
         <f t="shared" si="0"/>
-        <v>3.0999999999999996</v>
+        <v>5.9124999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1280,11 +1280,11 @@
       </c>
       <c r="G12">
         <f>+VLOOKUP(A12,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
+        <v>5.5</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1379,11 +1379,11 @@
       </c>
       <c r="G15">
         <f>+VLOOKUP(A15,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
+        <v>4.9732142857142856</v>
       </c>
       <c r="H15" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5.9866071428571423</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4140,7 +4140,7 @@
   <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4277,13 +4277,13 @@
       <c r="T2" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="U2" s="12" t="s">
         <v>143</v>
       </c>
       <c r="V2" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="W2" s="14" t="s">
+      <c r="W2" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4300,25 +4300,70 @@
         <f>+VLOOKUP(A3,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>MATTEO AVNDAÑO</v>
       </c>
-      <c r="I3">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3">
         <f>+(SUM(E3:H3)/SUM($E$1:$H$1))*6 + 1</f>
-        <v>1</v>
-      </c>
-      <c r="M3">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3" s="3">
         <f>+(SUM(J3:L3)/SUM($J$1:$L$1))*6 + 1</f>
-        <v>1</v>
-      </c>
-      <c r="Q3">
+        <v>7</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="3">
         <f>+(SUM(N3:P3)/SUM($N$1:$P$1))*6 + 1</f>
-        <v>1</v>
-      </c>
-      <c r="V3">
+        <v>7</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3" s="3">
         <f>+(SUM(R3:U3)/SUM($R$1:$U$1))*6 + 1</f>
         <v>1</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="3">
         <f>+I3*$I$1+M3*$M$1+Q3*$Q$1+V3*$V$1</f>
-        <v>1</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -4333,23 +4378,23 @@
         <f>+VLOOKUP(A4,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>YAÑEZ GALLEGOS</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <f t="shared" ref="I4:I19" si="0">+(SUM(E4:H4)/SUM($E$1:$H$1))*6 + 1</f>
         <v>1</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="3">
         <f t="shared" ref="M4:M19" si="1">+(SUM(J4:L4)/SUM($J$1:$L$1))*6 + 1</f>
         <v>1</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="3">
         <f t="shared" ref="Q4:Q19" si="2">+(SUM(N4:P4)/SUM($N$1:$P$1))*6 + 1</f>
         <v>1</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="3">
         <f t="shared" ref="V4:V19" si="3">+(SUM(R4:U4)/SUM($R$1:$U$1))*6 + 1</f>
         <v>1</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="3">
         <f t="shared" ref="W4:W19" si="4">+I4*$I$1+M4*$M$1+Q4*$Q$1+V4*$V$1</f>
         <v>1</v>
       </c>
@@ -4366,25 +4411,70 @@
         <f>+VLOOKUP(A5,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>QUIROZ LOPEZ</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M5">
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q5">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V5">
+        <v>6.1428571428571423</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W5">
+        <v>1.75</v>
+      </c>
+      <c r="W5" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.9732142857142856</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -4399,23 +4489,26 @@
         <f>+VLOOKUP(A6,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>CELEDON AGUIRRE</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M6">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M6" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -4432,25 +4525,70 @@
         <f>+VLOOKUP(A7,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>HINOJOSA BARRIGA</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M7">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q7">
+        <v>7</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V7">
+        <v>7</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7">
+        <v>2</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W7">
+        <v>5.5</v>
+      </c>
+      <c r="W7" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>6.625</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -4465,25 +4603,70 @@
         <f>+VLOOKUP(A8,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>ESTAY COLISTRO</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M8">
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q8">
+        <v>7</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V8">
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>2</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W8">
+        <v>4</v>
+      </c>
+      <c r="W8" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -4498,23 +4681,26 @@
         <f>+VLOOKUP(A9,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>BARROS AVILA</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M9">
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M9" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -4531,23 +4717,27 @@
         <f>+VLOOKUP(A10,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>LY CASTRO</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M10">
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="I10" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="W10">
+      <c r="W10" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -4564,23 +4754,23 @@
         <f>+VLOOKUP(A11,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>VERGARA PINUER</v>
       </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M11">
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M11" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="W11">
+      <c r="W11" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -4597,23 +4787,23 @@
         <f>+VLOOKUP(A12,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>CABELLO ALEGRIA</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M12">
+      <c r="I12" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M12" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="W12">
+      <c r="W12" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -4630,23 +4820,23 @@
         <f>+VLOOKUP(A13,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>RIVERA GUZMÁN</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M13">
+      <c r="I13" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M13" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="W13">
+      <c r="W13" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -4663,23 +4853,26 @@
         <f>+VLOOKUP(A14,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>CHAPARRO PEÑA</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M14">
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M14" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -4696,23 +4889,23 @@
         <f>+VLOOKUP(A15,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>PIMENTEL RAMIREZ</v>
       </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M15">
+      <c r="I15" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M15" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V15">
+      <c r="V15" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="W15">
+      <c r="W15" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -4729,23 +4922,23 @@
         <f>+VLOOKUP(A16,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>ARRIAZA TORO</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M16">
+      <c r="I16" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M16" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V16">
+      <c r="V16" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="W16">
+      <c r="W16" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -4762,23 +4955,23 @@
         <f>+VLOOKUP(A17,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>ARAOS GONZALEZ</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M17">
+      <c r="I17" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M17" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V17">
+      <c r="V17" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="W17">
+      <c r="W17" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -4795,23 +4988,26 @@
         <f>+VLOOKUP(A18,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>VALDES ALAMOS</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M18">
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M18" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V18">
+      <c r="V18" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="W18">
+      <c r="W18" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -4828,23 +5024,23 @@
         <f>+VLOOKUP(A19,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v xml:space="preserve">PARRA CONTRERAS </v>
       </c>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M19">
+      <c r="I19" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M19" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V19">
+      <c r="V19" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="W19">
+      <c r="W19" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
dmmd examen casi terminado
</commit_message>
<xml_diff>
--- a/Datos_Masivos/Verano_2023/ENGIN61901-2023A.xlsx
+++ b/Datos_Masivos/Verano_2023/ENGIN61901-2023A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andriu\Main\DOCUMENTOS\1. LABORALES\2. AYUDANTIAS\AyudantiasFEN\Datos_Masivos\Verano_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB34F48E-4059-4042-BE56-BBB47B57DEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A466EC0E-102B-400B-91EC-1B54021273D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{8460F878-2C6C-4FF6-8E48-E70BC54E4E5E}"/>
   </bookViews>
@@ -21,7 +21,8 @@
     <sheet name="EXAMEN" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">COMPILADO!$A$2:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">COMPILADO!$A$3:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">EXAMEN!$A$2:$W$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">LISTA!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="148">
   <si>
     <t>RUT</t>
   </si>
@@ -228,18 +229,6 @@
     <t>Microsoft Text Analytics</t>
   </si>
   <si>
-    <t>TAREA 1</t>
-  </si>
-  <si>
-    <t>TAREA 2</t>
-  </si>
-  <si>
-    <t>TAREA 3</t>
-  </si>
-  <si>
-    <t>EXAMEN</t>
-  </si>
-  <si>
     <t>referencial</t>
   </si>
   <si>
@@ -499,6 +488,30 @@
   </si>
   <si>
     <t>ACCIONES / IMPLEMENTAR</t>
+  </si>
+  <si>
+    <t>TAREA 2 - SQL</t>
+  </si>
+  <si>
+    <t>TAREA 3 - DASHBOARD</t>
+  </si>
+  <si>
+    <t>TAREA 1 - STATE OF ART</t>
+  </si>
+  <si>
+    <t>EXAMEN - SPARK</t>
+  </si>
+  <si>
+    <t>NOTA ANDRE</t>
+  </si>
+  <si>
+    <t>NOTA DAVID</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Andre</t>
   </si>
 </sst>
 </file>
@@ -508,7 +521,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,13 +551,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -559,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -573,7 +605,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -587,7 +618,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -903,619 +952,713 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D689BE8-E95D-44FE-B306-058F19D18108}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="J23" sqref="I23:J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D1" s="4"/>
+      <c r="E1" s="23">
         <v>0.5</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="5">
+      <c r="F1" s="23">
+        <v>0</v>
+      </c>
+      <c r="G1" s="23">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="H1" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="str">
-        <f>+VLOOKUP(A3,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>ARAOS GONZALEZ</v>
-      </c>
-      <c r="C3" t="str">
-        <f>+VLOOKUP(A3,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>ROBERTO ANDRES</v>
-      </c>
-      <c r="D3" s="3">
-        <f>+VLOOKUP(A3,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
-        <v>6</v>
-      </c>
-      <c r="E3" s="3">
-        <f>+VLOOKUP(A3,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
-        <v>7</v>
-      </c>
-      <c r="F3" s="3">
-        <f>+VLOOKUP(A3,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <f>+VLOOKUP(A3,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="H3" s="9">
-        <f>+E3*$E$1+G3*$G$1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
       </c>
       <c r="B4" t="str">
         <f>+VLOOKUP(A4,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>ARRIAZA TORO</v>
+        <v>ARAOS GONZALEZ</v>
       </c>
       <c r="C4" t="str">
         <f>+VLOOKUP(A4,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>PAULINA ADRIANA</v>
-      </c>
-      <c r="D4" s="3">
+        <v>ROBERTO ANDRES</v>
+      </c>
+      <c r="D4" s="21">
         <f>+VLOOKUP(A4,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="21">
         <f>+VLOOKUP(A4,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
-        <v>6.4</v>
-      </c>
-      <c r="F4" s="3">
+        <v>7</v>
+      </c>
+      <c r="F4" s="21">
         <f>+VLOOKUP(A4,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="21">
         <f>+VLOOKUP(A4,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="H4" s="9">
-        <f t="shared" ref="H4:H19" si="0">+E4*$E$1+G4*$G$1</f>
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H4" s="22">
+        <f>+E4*$E$1+G4*$G$1+F4*$F$1</f>
+        <v>5.5</v>
+      </c>
+      <c r="I4" s="22">
+        <f>+E4*$E$2+F4*$F$2+G4*$G$2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="str">
         <f>+VLOOKUP(A5,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>BARROS AVILA</v>
+        <v>ARRIAZA TORO</v>
       </c>
       <c r="C5" t="str">
         <f>+VLOOKUP(A5,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>FRANCISCA ANDREA</v>
-      </c>
-      <c r="D5" s="3">
+        <v>PAULINA ADRIANA</v>
+      </c>
+      <c r="D5" s="21">
         <f>+VLOOKUP(A5,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="E5" s="21">
+        <f>+VLOOKUP(A5,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
+        <v>6.4</v>
+      </c>
+      <c r="F5" s="21">
+        <f>+VLOOKUP(A5,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="E5" s="3">
-        <f>+VLOOKUP(A5,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
-        <v>5.8000000000000007</v>
-      </c>
-      <c r="F5" s="3">
-        <f>+VLOOKUP(A5,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="G5">
+      <c r="G5" s="21">
         <f>+VLOOKUP(A5,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="H5" s="9">
-        <f t="shared" si="0"/>
-        <v>3.4000000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3.5089285714285712</v>
+      </c>
+      <c r="H5" s="22">
+        <f t="shared" ref="H5:H20" si="0">+E5*$E$1+G5*$G$1+F5*$F$1</f>
+        <v>4.9544642857142858</v>
+      </c>
+      <c r="I5" s="22">
+        <f t="shared" ref="I5:I20" si="1">+E5*$E$2+F5*$F$2+G5*$G$2</f>
+        <v>4.6044642857142861</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="str">
         <f>+VLOOKUP(A6,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>CABELLO ALEGRIA</v>
+        <v>BARROS AVILA</v>
       </c>
       <c r="C6" t="str">
         <f>+VLOOKUP(A6,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>MARIO ULISES</v>
-      </c>
-      <c r="D6" s="3">
+        <v>FRANCISCA ANDREA</v>
+      </c>
+      <c r="D6" s="21">
         <f>+VLOOKUP(A6,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
-        <v>6</v>
-      </c>
-      <c r="E6" s="3">
+        <v>5</v>
+      </c>
+      <c r="E6" s="21">
         <f>+VLOOKUP(A6,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
-        <v>6.4</v>
-      </c>
-      <c r="F6" s="3">
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="F6" s="21">
         <f>+VLOOKUP(A6,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
-        <v>5.8000000000000007</v>
-      </c>
-      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="21">
         <f>+VLOOKUP(A6,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="H6" s="9">
-        <f t="shared" si="0"/>
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6.25</v>
+      </c>
+      <c r="H6" s="22">
+        <f t="shared" si="0"/>
+        <v>6.0250000000000004</v>
+      </c>
+      <c r="I6" s="22">
+        <f t="shared" si="1"/>
+        <v>4.8250000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="str">
         <f>+VLOOKUP(A7,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>CELEDON AGUIRRE</v>
+        <v>CABELLO ALEGRIA</v>
       </c>
       <c r="C7" t="str">
         <f>+VLOOKUP(A7,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>BASTIAN ANTONIO</v>
-      </c>
-      <c r="D7" s="3">
+        <v>MARIO ULISES</v>
+      </c>
+      <c r="D7" s="21">
         <f>+VLOOKUP(A7,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="21">
         <f>+VLOOKUP(A7,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
-        <v>7</v>
-      </c>
-      <c r="F7" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="F7" s="21">
         <f>+VLOOKUP(A7,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
-        <v>5.3999999999999995</v>
-      </c>
-      <c r="G7">
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="G7" s="21">
         <f>+VLOOKUP(A7,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="H7" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="H7" s="22">
+        <f t="shared" si="0"/>
+        <v>6.7</v>
+      </c>
+      <c r="I7" s="22">
+        <f t="shared" si="1"/>
+        <v>6.5500000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" t="str">
         <f>+VLOOKUP(A8,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>CHAPARRO PEÑA</v>
+        <v>CELEDON AGUIRRE</v>
       </c>
       <c r="C8" t="str">
         <f>+VLOOKUP(A8,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>PABLO</v>
-      </c>
-      <c r="D8" s="3">
+        <v>BASTIAN ANTONIO</v>
+      </c>
+      <c r="D8" s="21">
         <f>+VLOOKUP(A8,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="21">
         <f>+VLOOKUP(A8,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="21">
         <f>+VLOOKUP(A8,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
-        <v>5.8000000000000007</v>
-      </c>
-      <c r="G8">
+        <v>5.3999999999999995</v>
+      </c>
+      <c r="G8" s="21">
         <f>+VLOOKUP(A8,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="H8" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5.5</v>
+      </c>
+      <c r="H8" s="22">
+        <f t="shared" si="0"/>
+        <v>6.25</v>
+      </c>
+      <c r="I8" s="22">
+        <f t="shared" si="1"/>
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="str">
         <f>+VLOOKUP(A9,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>ESTAY COLISTRO</v>
+        <v>CHAPARRO PEÑA</v>
       </c>
       <c r="C9" t="str">
         <f>+VLOOKUP(A9,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>DANIEL ALEJANDRO</v>
-      </c>
-      <c r="D9" s="3">
+        <v>PABLO</v>
+      </c>
+      <c r="D9" s="21">
         <f>+VLOOKUP(A9,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="21">
         <f>+VLOOKUP(A9,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
-        <v>6.4</v>
-      </c>
-      <c r="F9" s="3">
+        <v>7</v>
+      </c>
+      <c r="F9" s="21">
         <f>+VLOOKUP(A9,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="G9">
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="G9" s="21">
         <f>+VLOOKUP(A9,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>6.25</v>
-      </c>
-      <c r="H9" s="9">
-        <f t="shared" si="0"/>
-        <v>6.3250000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6.625</v>
+      </c>
+      <c r="H9" s="22">
+        <f t="shared" si="0"/>
+        <v>6.8125</v>
+      </c>
+      <c r="I9" s="22">
+        <f t="shared" si="1"/>
+        <v>6.5125000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" t="str">
         <f>+VLOOKUP(A10,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>HINOJOSA BARRIGA</v>
+        <v>ESTAY COLISTRO</v>
       </c>
       <c r="C10" t="str">
         <f>+VLOOKUP(A10,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>CRISTIAN ANDRES</v>
-      </c>
-      <c r="D10" s="3">
+        <v>DANIEL ALEJANDRO</v>
+      </c>
+      <c r="D10" s="21">
         <f>+VLOOKUP(A10,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="21">
         <f>+VLOOKUP(A10,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
-        <v>5.1999999999999993</v>
-      </c>
-      <c r="F10" s="3">
+        <v>7</v>
+      </c>
+      <c r="F10" s="21">
         <f>+VLOOKUP(A10,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
-        <v>6.6</v>
-      </c>
-      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="G10" s="21">
         <f>+VLOOKUP(A10,EXAMEN!$A$3:$W$19,23,FALSE)</f>
+        <v>6.25</v>
+      </c>
+      <c r="H10" s="22">
+        <f t="shared" si="0"/>
         <v>6.625</v>
       </c>
-      <c r="H10" s="9">
-        <f t="shared" si="0"/>
-        <v>5.9124999999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="22">
+        <f t="shared" si="1"/>
+        <v>6.125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11" t="str">
         <f>+VLOOKUP(A11,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>LY CASTRO</v>
+        <v>HINOJOSA BARRIGA</v>
       </c>
       <c r="C11" t="str">
         <f>+VLOOKUP(A11,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>JUAN FELIPE ANDRÉS</v>
-      </c>
-      <c r="D11" s="3">
+        <v>CRISTIAN ANDRES</v>
+      </c>
+      <c r="D11" s="21">
         <f>+VLOOKUP(A11,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="21">
         <f>+VLOOKUP(A11,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
         <v>5.8000000000000007</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="21">
         <f>+VLOOKUP(A11,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="G11">
+        <v>6.6</v>
+      </c>
+      <c r="G11" s="21">
         <f>+VLOOKUP(A11,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="H11" s="9">
-        <f t="shared" si="0"/>
-        <v>3.4000000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6.625</v>
+      </c>
+      <c r="H11" s="22">
+        <f t="shared" si="0"/>
+        <v>6.2125000000000004</v>
+      </c>
+      <c r="I11" s="22">
+        <f t="shared" si="1"/>
+        <v>6.4124999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" t="str">
         <f>+VLOOKUP(A12,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>MATTEO AVNDAÑO</v>
+        <v>LY CASTRO</v>
       </c>
       <c r="C12" t="str">
         <f>+VLOOKUP(A12,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>ALONSO NICOLÁS</v>
-      </c>
-      <c r="D12" s="3">
+        <v>JUAN FELIPE ANDRÉS</v>
+      </c>
+      <c r="D12" s="21">
         <f>+VLOOKUP(A12,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="21">
         <f>+VLOOKUP(A12,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
-        <v>7</v>
-      </c>
-      <c r="F12" s="3">
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="F12" s="21">
         <f>+VLOOKUP(A12,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
-        <v>5.8000000000000007</v>
-      </c>
-      <c r="G12">
+        <v>3.8</v>
+      </c>
+      <c r="G12" s="21">
         <f>+VLOOKUP(A12,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>5.5</v>
-      </c>
-      <c r="H12" s="9">
-        <f t="shared" si="0"/>
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4.8125</v>
+      </c>
+      <c r="H12" s="22">
+        <f t="shared" si="0"/>
+        <v>5.3062500000000004</v>
+      </c>
+      <c r="I12" s="22">
+        <f t="shared" si="1"/>
+        <v>4.8062500000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>22</v>
       </c>
       <c r="B13" t="str">
         <f>+VLOOKUP(A13,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v xml:space="preserve">PARRA CONTRERAS </v>
+        <v>MATTEO AVNDAÑO</v>
       </c>
       <c r="C13" t="str">
         <f>+VLOOKUP(A13,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>SEBASTIÁN GERARDO</v>
-      </c>
-      <c r="D13" s="3">
+        <v>ALONSO NICOLÁS</v>
+      </c>
+      <c r="D13" s="21">
         <f>+VLOOKUP(A13,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="21">
         <f>+VLOOKUP(A13,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
-        <v>5.8000000000000007</v>
-      </c>
-      <c r="F13" s="3">
+        <v>7</v>
+      </c>
+      <c r="F13" s="21">
         <f>+VLOOKUP(A13,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
         <v>5.8000000000000007</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="21">
         <f>+VLOOKUP(A13,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="H13" s="9">
-        <f t="shared" si="0"/>
-        <v>3.4000000000000004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5.5</v>
+      </c>
+      <c r="H13" s="22">
+        <f t="shared" si="0"/>
+        <v>6.25</v>
+      </c>
+      <c r="I13" s="22">
+        <f t="shared" si="1"/>
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="B14" t="str">
         <f>+VLOOKUP(A14,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>PIMENTEL RAMIREZ</v>
+        <v xml:space="preserve">PARRA CONTRERAS </v>
       </c>
       <c r="C14" t="str">
         <f>+VLOOKUP(A14,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>PATRICIO IVAN</v>
-      </c>
-      <c r="D14" s="3">
+        <v>SEBASTIÁN GERARDO</v>
+      </c>
+      <c r="D14" s="21">
         <f>+VLOOKUP(A14,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="21">
         <f>+VLOOKUP(A14,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
-        <v>7</v>
-      </c>
-      <c r="F14" s="3">
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="F14" s="21">
         <f>+VLOOKUP(A14,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
-        <v>5.3999999999999995</v>
-      </c>
-      <c r="G14">
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="G14" s="21">
         <f>+VLOOKUP(A14,EXAMEN!$A$3:$W$19,23,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="H14" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="22">
+        <f t="shared" si="0"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="I14" s="22">
+        <f t="shared" si="1"/>
+        <v>3.4000000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B15" t="str">
         <f>+VLOOKUP(A15,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>QUIROZ LOPEZ</v>
+        <v>PIMENTEL RAMIREZ</v>
       </c>
       <c r="C15" t="str">
         <f>+VLOOKUP(A15,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>ANIBAL IGOR</v>
-      </c>
-      <c r="D15" s="3">
+        <v>PATRICIO IVAN</v>
+      </c>
+      <c r="D15" s="21">
         <f>+VLOOKUP(A15,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="E15" s="3">
+        <v>6</v>
+      </c>
+      <c r="E15" s="21">
         <f>+VLOOKUP(A15,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="21">
         <f>+VLOOKUP(A15,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
+        <v>5.3999999999999995</v>
+      </c>
+      <c r="G15" s="21">
+        <f>+VLOOKUP(A15,EXAMEN!$A$3:$W$19,23,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="H15" s="22">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I15" s="22">
+        <f t="shared" si="1"/>
         <v>6.6</v>
       </c>
-      <c r="G15">
-        <f>+VLOOKUP(A15,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>4.9732142857142856</v>
-      </c>
-      <c r="H15" s="9">
-        <f t="shared" si="0"/>
-        <v>5.9866071428571423</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" t="str">
         <f>+VLOOKUP(A16,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>RIVERA GUZMÁN</v>
+        <v>QUIROZ LOPEZ</v>
       </c>
       <c r="C16" t="str">
         <f>+VLOOKUP(A16,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>PABLO ANDRÉS</v>
-      </c>
-      <c r="D16" s="3">
+        <v>ANIBAL IGOR</v>
+      </c>
+      <c r="D16" s="21">
         <f>+VLOOKUP(A16,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="21">
         <f>+VLOOKUP(A16,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="21">
         <f>+VLOOKUP(A16,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
-        <v>4.2</v>
-      </c>
-      <c r="G16">
+        <v>6.6</v>
+      </c>
+      <c r="G16" s="21">
         <f>+VLOOKUP(A16,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="H16" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4.9732142857142856</v>
+      </c>
+      <c r="H16" s="22">
+        <f t="shared" si="0"/>
+        <v>5.9866071428571423</v>
+      </c>
+      <c r="I16" s="22">
+        <f t="shared" si="1"/>
+        <v>5.8866071428571427</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" t="str">
         <f>+VLOOKUP(A17,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>VALDES ALAMOS</v>
+        <v>RIVERA GUZMÁN</v>
       </c>
       <c r="C17" t="str">
         <f>+VLOOKUP(A17,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>RODRIGO ALEJANDRO</v>
-      </c>
-      <c r="D17" s="3">
+        <v>PABLO ANDRÉS</v>
+      </c>
+      <c r="D17" s="21">
         <f>+VLOOKUP(A17,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
-        <v>6</v>
-      </c>
-      <c r="E17" s="3">
+        <v>5</v>
+      </c>
+      <c r="E17" s="21">
         <f>+VLOOKUP(A17,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
-        <v>5.1999999999999993</v>
-      </c>
-      <c r="F17" s="3">
+        <v>7</v>
+      </c>
+      <c r="F17" s="21">
         <f>+VLOOKUP(A17,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
         <v>4.2</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="21">
         <f>+VLOOKUP(A17,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="H17" s="9">
-        <f t="shared" si="0"/>
-        <v>3.0999999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="H17" s="22">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I17" s="22">
+        <f t="shared" si="1"/>
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" t="str">
         <f>+VLOOKUP(A18,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>VERGARA PINUER</v>
+        <v>VALDES ALAMOS</v>
       </c>
       <c r="C18" t="str">
         <f>+VLOOKUP(A18,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>JUAN PABLO</v>
-      </c>
-      <c r="D18" s="3">
+        <v>RODRIGO ALEJANDRO</v>
+      </c>
+      <c r="D18" s="21">
         <f>+VLOOKUP(A18,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="E18" s="3">
+        <v>6</v>
+      </c>
+      <c r="E18" s="21">
         <f>+VLOOKUP(A18,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
-        <v>6.4</v>
-      </c>
-      <c r="F18" s="3">
+        <v>5.1999999999999993</v>
+      </c>
+      <c r="F18" s="21">
         <f>+VLOOKUP(A18,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
-        <v>6.2</v>
-      </c>
-      <c r="G18">
+        <v>4.2</v>
+      </c>
+      <c r="G18" s="21">
         <f>+VLOOKUP(A18,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="H18" s="9">
-        <f t="shared" si="0"/>
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4.9732142857142856</v>
+      </c>
+      <c r="H18" s="22">
+        <f t="shared" si="0"/>
+        <v>5.086607142857142</v>
+      </c>
+      <c r="I18" s="22">
+        <f t="shared" si="1"/>
+        <v>4.836607142857142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" t="str">
         <f>+VLOOKUP(A19,LISTA!$A$2:$E$18,3,FALSE)</f>
-        <v>YAÑEZ GALLEGOS</v>
+        <v>VERGARA PINUER</v>
       </c>
       <c r="C19" t="str">
         <f>+VLOOKUP(A19,LISTA!$A$2:$E$18,2,FALSE)</f>
-        <v>ANDREA VERONICA</v>
-      </c>
-      <c r="D19" s="3">
+        <v>JUAN PABLO</v>
+      </c>
+      <c r="D19" s="21">
         <f>+VLOOKUP(A19,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="21">
         <f>+VLOOKUP(A19,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
-        <v>7</v>
-      </c>
-      <c r="F19" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="F19" s="21">
         <f>+VLOOKUP(A19,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
+        <v>6.2</v>
+      </c>
+      <c r="G19" s="21">
+        <f>+VLOOKUP(A19,EXAMEN!$A$3:$W$19,23,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="H19" s="22">
+        <f t="shared" si="0"/>
+        <v>6.7</v>
+      </c>
+      <c r="I19" s="22">
+        <f t="shared" si="1"/>
+        <v>6.65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="str">
+        <f>+VLOOKUP(A20,LISTA!$A$2:$E$18,3,FALSE)</f>
+        <v>YAÑEZ GALLEGOS</v>
+      </c>
+      <c r="C20" t="str">
+        <f>+VLOOKUP(A20,LISTA!$A$2:$E$18,2,FALSE)</f>
+        <v>ANDREA VERONICA</v>
+      </c>
+      <c r="D20" s="21">
+        <f>+VLOOKUP(A20,'TAREA 1'!$A$3:$K$19,11,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="E20" s="21">
+        <f>+VLOOKUP(A20,'TAREA 2'!$A$3:$K$19,11,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="F20" s="21">
+        <f>+VLOOKUP(A20,'TAREA 3'!$A$3:$N$19,14,FALSE)</f>
         <v>5.3999999999999995</v>
       </c>
-      <c r="G19">
-        <f>+VLOOKUP(A19,EXAMEN!$A$3:$W$19,23,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="H19" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
+      <c r="G20" s="21">
+        <f>+VLOOKUP(A20,EXAMEN!$A$3:$W$19,23,FALSE)</f>
+        <v>4.9464285714285712</v>
+      </c>
+      <c r="H20" s="22">
+        <f t="shared" si="0"/>
+        <v>5.9732142857142856</v>
+      </c>
+      <c r="I20" s="22">
+        <f t="shared" si="1"/>
+        <v>5.5732142857142852</v>
       </c>
     </row>
   </sheetData>
@@ -1546,10 +1689,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1563,16 +1706,16 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1580,16 +1723,16 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1597,16 +1740,16 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1614,16 +1757,16 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1631,16 +1774,16 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1648,16 +1791,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1665,16 +1808,16 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1682,16 +1825,16 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1699,16 +1842,16 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
         <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1716,16 +1859,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1733,16 +1876,16 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
         <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1750,16 +1893,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1767,16 +1910,16 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1784,16 +1927,16 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1801,16 +1944,16 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1818,33 +1961,33 @@
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
         <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D18" t="s">
         <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1894,10 +2037,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>37</v>
@@ -2579,7 +2722,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2615,31 +2758,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="J2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>43</v>
@@ -2814,7 +2957,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -2833,7 +2976,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>5.1999999999999993</v>
+        <v>5.8000000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2852,7 +2995,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -2871,7 +3014,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>6.4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3302,7 +3445,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3345,40 +3488,40 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>43</v>
@@ -3668,21 +3811,30 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
+      <c r="A9" s="16" t="str">
         <v>18.536.954-4</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="16" t="str">
         <f>+VLOOKUP(A9,'TAREA 1'!$A$3:$K$19,2,FALSE)</f>
         <v>FRANCISCA ANDREA</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="16" t="str">
         <f>+VLOOKUP(A9,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>BARROS AVILA</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="N9" s="3">
+      <c r="D9" s="16">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="17">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3700,11 +3852,38 @@
         <v>LY CASTRO</v>
       </c>
       <c r="D10">
-        <v>-1</v>
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -4139,8 +4318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FC8862-8EFF-4404-A963-EBA68A6AD34F}">
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4217,73 +4396,73 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="J2" s="11" t="s">
+      <c r="O2" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="P2" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="R2" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="N2" s="11" t="s">
+      <c r="T2" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="U2" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="P2" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="W2" s="13" t="s">
+      <c r="V2" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="W2" s="12" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4378,25 +4557,70 @@
         <f>+VLOOKUP(A4,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>YAÑEZ GALLEGOS</v>
       </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
       <c r="I4" s="3">
         <f t="shared" ref="I4:I19" si="0">+(SUM(E4:H4)/SUM($E$1:$H$1))*6 + 1</f>
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
         <v>1</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" ref="M4:M19" si="1">+(SUM(J4:L4)/SUM($J$1:$L$1))*6 + 1</f>
-        <v>1</v>
+        <f>+(SUM(J4:L4)/SUM($J$1:$L$1))*6 + 1</f>
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
       </c>
       <c r="Q4" s="3">
-        <f t="shared" ref="Q4:Q19" si="2">+(SUM(N4:P4)/SUM($N$1:$P$1))*6 + 1</f>
-        <v>1</v>
+        <f t="shared" ref="Q4:Q19" si="1">+(SUM(N4:P4)/SUM($N$1:$P$1))*6 + 1</f>
+        <v>5.2857142857142856</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
       </c>
       <c r="V4" s="3">
-        <f t="shared" ref="V4:V19" si="3">+(SUM(R4:U4)/SUM($R$1:$U$1))*6 + 1</f>
-        <v>1</v>
+        <f t="shared" ref="V4:V19" si="2">+(SUM(R4:U4)/SUM($R$1:$U$1))*6 + 1</f>
+        <v>2.5</v>
       </c>
       <c r="W4" s="3">
-        <f t="shared" ref="W4:W19" si="4">+I4*$I$1+M4*$M$1+Q4*$Q$1+V4*$V$1</f>
-        <v>1</v>
+        <f t="shared" ref="W4:W19" si="3">+I4*$I$1+M4*$M$1+Q4*$Q$1+V4*$V$1</f>
+        <v>4.9464285714285712</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -4440,40 +4664,40 @@
         <v>1</v>
       </c>
       <c r="M5" s="3">
+        <f t="shared" ref="M5:M19" si="4">+(SUM(J5:L5)/SUM($J$1:$L$1))*6 + 1</f>
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="3">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="N5">
-        <v>2</v>
-      </c>
-      <c r="O5">
-        <v>2</v>
-      </c>
-      <c r="P5">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="3">
+        <v>6.1428571428571423</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5" s="3">
         <f t="shared" si="2"/>
-        <v>6.1428571428571423</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="W5" s="3">
         <f t="shared" si="3"/>
-        <v>1.75</v>
-      </c>
-      <c r="W5" s="3">
-        <f t="shared" si="4"/>
         <v>4.9732142857142856</v>
       </c>
     </row>
@@ -4492,25 +4716,67 @@
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
       <c r="I6" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
       </c>
       <c r="M6" s="3">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q6" s="3">
+        <v>7</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V6" s="3">
+      <c r="W6" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W6" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -4554,7 +4820,7 @@
         <v>2</v>
       </c>
       <c r="M7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="N7">
@@ -4567,27 +4833,27 @@
         <v>2</v>
       </c>
       <c r="Q7" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7">
+        <v>2</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7" s="3">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="R7">
-        <v>2</v>
-      </c>
-      <c r="S7">
-        <v>2</v>
-      </c>
-      <c r="T7">
-        <v>2</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="W7" s="3">
         <f t="shared" si="3"/>
-        <v>5.5</v>
-      </c>
-      <c r="W7" s="3">
-        <f t="shared" si="4"/>
         <v>6.625</v>
       </c>
     </row>
@@ -4632,7 +4898,7 @@
         <v>2</v>
       </c>
       <c r="M8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="N8">
@@ -4645,27 +4911,27 @@
         <v>2</v>
       </c>
       <c r="Q8" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>2</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8" s="3">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>1</v>
-      </c>
-      <c r="T8">
-        <v>2</v>
-      </c>
-      <c r="U8">
-        <v>1</v>
-      </c>
-      <c r="V8" s="3">
+        <v>4</v>
+      </c>
+      <c r="W8" s="3">
         <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="W8" s="3">
-        <f t="shared" si="4"/>
         <v>6.25</v>
       </c>
     </row>
@@ -4684,25 +4950,67 @@
       <c r="D9">
         <v>3</v>
       </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
       <c r="I9" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
       </c>
       <c r="M9" s="3">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q9" s="3">
+        <v>7</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>2</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V9" s="3">
+        <v>4</v>
+      </c>
+      <c r="W9" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W9" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -4720,26 +5028,67 @@
       <c r="D10">
         <v>5</v>
       </c>
-      <c r="G10" s="14"/>
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13">
+        <v>2</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>2</v>
+      </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="J10" s="13">
+        <v>2</v>
+      </c>
+      <c r="K10" s="13">
+        <v>1</v>
+      </c>
+      <c r="L10" s="13">
         <v>1</v>
       </c>
       <c r="M10" s="3">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="N10" s="13">
+        <v>3</v>
+      </c>
+      <c r="O10" s="13">
+        <v>2</v>
+      </c>
+      <c r="P10" s="13">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q10" s="3">
+        <v>7</v>
+      </c>
+      <c r="R10" s="13">
+        <v>1</v>
+      </c>
+      <c r="S10" s="13">
+        <v>0</v>
+      </c>
+      <c r="T10" s="13">
+        <v>0</v>
+      </c>
+      <c r="U10" s="13">
+        <v>0</v>
+      </c>
+      <c r="V10" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V10" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="W10" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W10" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.8125</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -4754,25 +5103,70 @@
         <f>+VLOOKUP(A11,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>VERGARA PINUER</v>
       </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
       <c r="I11" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
       </c>
       <c r="M11" s="3">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q11" s="3">
+        <v>7</v>
+      </c>
+      <c r="R11">
+        <v>2</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>2</v>
+      </c>
+      <c r="U11">
+        <v>2</v>
+      </c>
+      <c r="V11" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V11" s="3">
+        <v>7</v>
+      </c>
+      <c r="W11" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W11" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -4787,25 +5181,70 @@
         <f>+VLOOKUP(A12,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>CABELLO ALEGRIA</v>
       </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
       <c r="I12" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
       </c>
       <c r="M12" s="3">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q12" s="3">
+        <v>7</v>
+      </c>
+      <c r="R12">
+        <v>2</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="T12">
+        <v>2</v>
+      </c>
+      <c r="U12">
+        <v>2</v>
+      </c>
+      <c r="V12" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V12" s="3">
+        <v>7</v>
+      </c>
+      <c r="W12" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W12" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -4820,25 +5259,70 @@
         <f>+VLOOKUP(A13,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>RIVERA GUZMÁN</v>
       </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
       <c r="I13" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
       </c>
       <c r="M13" s="3">
+        <f>+(SUM(J13:L13)/SUM($J$1:$L$1))*6 + 1</f>
+        <v>7</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q13" s="3">
+        <v>7</v>
+      </c>
+      <c r="R13">
+        <v>2</v>
+      </c>
+      <c r="S13">
+        <v>2</v>
+      </c>
+      <c r="T13">
+        <v>2</v>
+      </c>
+      <c r="U13">
+        <v>2</v>
+      </c>
+      <c r="V13" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V13" s="3">
+        <v>7</v>
+      </c>
+      <c r="W13" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W13" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -4856,25 +5340,67 @@
       <c r="D14">
         <v>2</v>
       </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
       <c r="I14" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
       </c>
       <c r="M14" s="3">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q14" s="3">
+        <v>7</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
+      <c r="S14">
+        <v>2</v>
+      </c>
+      <c r="T14">
+        <v>2</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V14" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="W14" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W14" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <v>6.625</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -4889,25 +5415,70 @@
         <f>+VLOOKUP(A15,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>PIMENTEL RAMIREZ</v>
       </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
       <c r="I15" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
       </c>
       <c r="M15" s="3">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="N15">
+        <v>3</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q15" s="3">
+        <v>7</v>
+      </c>
+      <c r="R15">
+        <v>2</v>
+      </c>
+      <c r="S15">
+        <v>2</v>
+      </c>
+      <c r="T15">
+        <v>2</v>
+      </c>
+      <c r="U15">
+        <v>2</v>
+      </c>
+      <c r="V15" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V15" s="3">
+        <v>7</v>
+      </c>
+      <c r="W15" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W15" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -4922,58 +5493,134 @@
         <f>+VLOOKUP(A16,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>ARRIAZA TORO</v>
       </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
       <c r="I16" s="3">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
         <v>1</v>
       </c>
       <c r="M16" s="3">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>3</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q16" s="3">
+        <v>5.2857142857142856</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V16" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="W16" s="14">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W16" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3.5089285714285712</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
+      <c r="A17" s="15" t="str">
         <v>14.576.512-9</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B17" s="15" t="str">
         <f>+VLOOKUP(A17,'TAREA 1'!$A$3:$K$19,2,FALSE)</f>
         <v>ROBERTO ANDRES</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="15" t="str">
         <f>+VLOOKUP(A17,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v>ARAOS GONZALEZ</v>
       </c>
-      <c r="I17" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M17" s="3">
+      <c r="D17" s="15">
+        <v>9</v>
+      </c>
+      <c r="E17" s="15">
+        <v>2</v>
+      </c>
+      <c r="F17" s="15">
+        <v>2</v>
+      </c>
+      <c r="G17" s="15">
+        <v>2</v>
+      </c>
+      <c r="H17" s="15">
+        <v>2</v>
+      </c>
+      <c r="I17" s="19">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J17" s="15">
+        <v>2</v>
+      </c>
+      <c r="K17" s="15">
+        <v>2</v>
+      </c>
+      <c r="L17" s="15">
+        <v>2</v>
+      </c>
+      <c r="M17" s="19">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="19">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V17" s="3">
+      <c r="W17" s="19">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W17" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -4991,61 +5638,121 @@
       <c r="D18">
         <v>4</v>
       </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
       <c r="I18" s="3">
         <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
         <v>1</v>
       </c>
       <c r="M18" s="3">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q18" s="3">
+        <v>6.1428571428571423</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V18" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="W18" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W18" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4.9732142857142856</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
+      <c r="A19" s="16" t="str">
         <v>17.704.178-5</v>
       </c>
-      <c r="B19" t="str">
+      <c r="B19" s="16" t="str">
         <f>+VLOOKUP(A19,'TAREA 1'!$A$3:$K$19,2,FALSE)</f>
         <v>SEBASTIÁN GERARDO</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C19" s="16" t="str">
         <f>+VLOOKUP(A19,'TAREA 1'!$A$3:$K$19,3,FALSE)</f>
         <v xml:space="preserve">PARRA CONTRERAS </v>
       </c>
-      <c r="I19" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M19" s="3">
+      <c r="D19" s="16">
+        <v>-1</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="17">
+        <f>+(SUM(E19:H19)/SUM($E$1:$H$1))*6 + 1</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="17">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="17">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="17">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V19" s="3">
+      <c r="W19" s="18">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="W19" s="3">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>